<commit_message>
Added reports upload feature
</commit_message>
<xml_diff>
--- a/189.xlsx
+++ b/189.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artyom\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12223BB2-0ABE-4F0E-A47E-1995AEB29843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921FCA09-DDB7-40E5-9424-984EC6800164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Слово</t>
   </si>
@@ -39,25 +39,59 @@
     <t>Переклад</t>
   </si>
   <si>
-    <t>hhfhf</t>
-  </si>
-  <si>
-    <t>geeyy</t>
-  </si>
-  <si>
-    <t>hff</t>
+    <t>Англійська</t>
+  </si>
+  <si>
+    <t>Прикметник</t>
+  </si>
+  <si>
+    <t>блискучий, сяйливий, лискучий</t>
+  </si>
+  <si>
+    <t>Прийменник</t>
+  </si>
+  <si>
+    <t>з, від</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>ухх, тест, теса</t>
+  </si>
+  <si>
+    <t>shind</t>
+  </si>
+  <si>
+    <t>dd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -81,8 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -363,42 +399,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="85.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>